<commit_message>
OW-438 updated the excel test files following the feature branch merge
</commit_message>
<xml_diff>
--- a/src/test/resources/portfolio/OneFX.xlsx
+++ b/src/test/resources/portfolio/OneFX.xlsx
@@ -29,7 +29,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="115">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -270,9 +270,6 @@
     <t xml:space="preserve">LEG2_VARIABLECURRENCY</t>
   </si>
   <si>
-    <t xml:space="preserve">Value_Date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Position_Account_ID</t>
   </si>
   <si>
@@ -348,12 +345,15 @@
     <t xml:space="preserve">201000</t>
   </si>
   <si>
+    <t xml:space="preserve">2017/06/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00:00.000</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017/06/14</t>
   </si>
   <si>
-    <t xml:space="preserve">12:00:00.000</t>
-  </si>
-  <si>
     <t xml:space="preserve">BILATERAL</t>
   </si>
   <si>
@@ -372,16 +372,16 @@
     <t xml:space="preserve">0.97</t>
   </si>
   <si>
+    <t xml:space="preserve">2017/06/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModifiedFollowing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHZU</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017/06/19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModifiedFollowing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHZU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017/06/21</t>
   </si>
   <si>
     <t xml:space="preserve">CHF</t>
@@ -451,18 +451,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -516,7 +510,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,59 +547,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="51" min="50" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="51" min="50" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="57" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,49 +797,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,60 +1007,61 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="52" min="51" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="52" min="51" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="58" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,49 +1261,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,248 +1463,265 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.72959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.25"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.69387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.07142857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.54081632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.25"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6071428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.4591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.1938775510204"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="34.1275510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.6581632653061"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="34.2448979591837"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="22.7755102040816"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.3214285714286"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.25"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.7551020408163"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6071428571429"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.4591836734694"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.1938775510204"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="34.1275510204082"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="22.6581632653061"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="34.2448979591837"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.7755102040816"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="23.1275510204082"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.6173469387755"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="10.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="0" t="s">
+      <c r="K1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="W1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AC1" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AD1" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AE1" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AF1" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AG1" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="AF1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AH1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AI1" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AJ1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AK1" s="0" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>999</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="U2" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Z2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AC2" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AD2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="AF2" s="0" t="s">
+      <c r="AG2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AH2" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AI2" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="AI2" s="0" t="s">
+      <c r="AJ2" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="AJ2" s="0" t="s">
+      <c r="AK2" s="0" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>